<commit_message>
fix bug thanh toan
</commit_message>
<xml_diff>
--- a/Excel/order_statistics.xlsx
+++ b/Excel/order_statistics.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R1cef7769a4544dbc"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R4b48aa40fa754e55"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -29,10 +29,10 @@
         <x:v>Lê Huỳnh Phát</x:v>
       </x:c>
       <x:c>
-        <x:v>168000</x:v>
+        <x:v>516000</x:v>
       </x:c>
       <x:c>
-        <x:v>2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c>
         <x:v>05/10/2023</x:v>

</xml_diff>